<commit_message>
Update Control de Correspondencia año 2022 (Autoguardado).xlsx
</commit_message>
<xml_diff>
--- a/Control de Correspondencia año 2022 (Autoguardado).xlsx
+++ b/Control de Correspondencia año 2022 (Autoguardado).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teresa Andino\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teresa Andino\Documents\GitHub\Matrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0877D33-E4F9-4253-B660-ADF8D2647FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7407DAAD-96D6-4800-A306-14ABEC3DAA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>No. de Oficio</t>
   </si>
@@ -297,6 +297,31 @@
   </si>
   <si>
     <t>Oficio No. 2701-ETNEM-SS-2024</t>
+  </si>
+  <si>
+    <t>Oficio No. 1105-DGRP-2024</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Por este medio solicito se realice el tramite adaministrativo  para lanzar el proceso de las compras de formulaPolimerica nutricionalmente completa y balanceada, esta actividad esta esta enmarcada en el presupuesto asignado al pla para fortalecimiento y la sostenibilidad de las 3 subvenciones en </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>el objeto de gasto 31110 Alimentos y Bebidas.</t>
+    </r>
+  </si>
+  <si>
+    <t>Dr. Saul Herna Cruz</t>
+  </si>
+  <si>
+    <t>se le pasa a Jessy para respuesta</t>
   </si>
 </sst>
 </file>
@@ -807,6 +832,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -836,15 +870,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1152,8 +1177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L3215"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,26 +1193,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="2:8" ht="47.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
     </row>
     <row r="3" spans="2:8" ht="47.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
@@ -1213,7 +1238,7 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="55" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="3">
@@ -1234,7 +1259,7 @@
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="56" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="10">
@@ -1257,7 +1282,7 @@
       </c>
     </row>
     <row r="6" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="56" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="10">
@@ -1280,7 +1305,7 @@
       </c>
     </row>
     <row r="7" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="57" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="10">
@@ -1303,7 +1328,7 @@
       </c>
     </row>
     <row r="8" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="56" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="10">
@@ -1326,7 +1351,7 @@
       </c>
     </row>
     <row r="9" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="56" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="10">
@@ -1348,14 +1373,28 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="15"/>
+    <row r="10" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B10" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="10">
+        <v>45467</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="16"/>
@@ -4181,13 +4220,13 @@
       <c r="H323" s="27"/>
     </row>
     <row r="324" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B324" s="62"/>
-      <c r="C324" s="63"/>
-      <c r="D324" s="63"/>
-      <c r="E324" s="63"/>
-      <c r="F324" s="63"/>
-      <c r="G324" s="63"/>
-      <c r="H324" s="64"/>
+      <c r="B324" s="65"/>
+      <c r="C324" s="66"/>
+      <c r="D324" s="66"/>
+      <c r="E324" s="66"/>
+      <c r="F324" s="66"/>
+      <c r="G324" s="66"/>
+      <c r="H324" s="67"/>
     </row>
     <row r="325" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B325" s="34"/>
@@ -4259,7 +4298,7 @@
       <c r="E332" s="31"/>
       <c r="F332" s="32"/>
       <c r="G332" s="33"/>
-      <c r="H332" s="57"/>
+      <c r="H332" s="60"/>
     </row>
     <row r="333" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B333" s="34"/>
@@ -4268,7 +4307,7 @@
       <c r="E333" s="31"/>
       <c r="F333" s="32"/>
       <c r="G333" s="33"/>
-      <c r="H333" s="58"/>
+      <c r="H333" s="61"/>
     </row>
     <row r="334" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B334" s="34"/>
@@ -4277,7 +4316,7 @@
       <c r="E334" s="31"/>
       <c r="F334" s="32"/>
       <c r="G334" s="33"/>
-      <c r="H334" s="59"/>
+      <c r="H334" s="62"/>
     </row>
     <row r="335" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B335" s="34"/>
@@ -4682,7 +4721,7 @@
       <c r="E379" s="31"/>
       <c r="F379" s="32"/>
       <c r="G379" s="33"/>
-      <c r="H379" s="57"/>
+      <c r="H379" s="60"/>
     </row>
     <row r="380" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B380" s="34"/>
@@ -4691,7 +4730,7 @@
       <c r="E380" s="31"/>
       <c r="F380" s="32"/>
       <c r="G380" s="33"/>
-      <c r="H380" s="59"/>
+      <c r="H380" s="62"/>
     </row>
     <row r="381" spans="2:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B381" s="34"/>
@@ -4736,7 +4775,7 @@
       <c r="E385" s="31"/>
       <c r="F385" s="32"/>
       <c r="G385" s="33"/>
-      <c r="H385" s="57"/>
+      <c r="H385" s="60"/>
     </row>
     <row r="386" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B386" s="34"/>
@@ -4745,7 +4784,7 @@
       <c r="E386" s="31"/>
       <c r="F386" s="32"/>
       <c r="G386" s="33"/>
-      <c r="H386" s="58"/>
+      <c r="H386" s="61"/>
     </row>
     <row r="387" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B387" s="34"/>
@@ -4754,7 +4793,7 @@
       <c r="E387" s="31"/>
       <c r="F387" s="32"/>
       <c r="G387" s="33"/>
-      <c r="H387" s="59"/>
+      <c r="H387" s="62"/>
     </row>
     <row r="388" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B388" s="34"/>
@@ -5951,7 +5990,7 @@
       <c r="E520" s="22"/>
       <c r="F520" s="22"/>
       <c r="G520" s="22"/>
-      <c r="H520" s="55"/>
+      <c r="H520" s="58"/>
     </row>
     <row r="521" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B521" s="22"/>
@@ -5960,7 +5999,7 @@
       <c r="E521" s="22"/>
       <c r="F521" s="22"/>
       <c r="G521" s="22"/>
-      <c r="H521" s="56"/>
+      <c r="H521" s="59"/>
     </row>
     <row r="522" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B522" s="22"/>

</xml_diff>